<commit_message>
📊 Update NAIC content history - 2025-12-02
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm20-table-j-swaps.xlsx
+++ b/docs/content_history/pbr-2025-vm20-table-j-swaps.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4990BA3-39B1-4108-9318-0247D4456070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134B07F-FBD7-404A-925A-14D24D59845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="2595" windowWidth="26490" windowHeight="11010" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="October_2025" sheetId="26" r:id="rId1"/>
-    <sheet name="September_2025" sheetId="25" r:id="rId2"/>
-    <sheet name="August_2025" sheetId="24" r:id="rId3"/>
-    <sheet name="July_2025" sheetId="23" r:id="rId4"/>
-    <sheet name="June_2025" sheetId="22" r:id="rId5"/>
-    <sheet name="May_2025" sheetId="21" r:id="rId6"/>
-    <sheet name="April_2025" sheetId="20" r:id="rId7"/>
-    <sheet name="March_2025" sheetId="19" r:id="rId8"/>
-    <sheet name="February_2025" sheetId="18" r:id="rId9"/>
-    <sheet name="January_2025" sheetId="17" r:id="rId10"/>
-    <sheet name="LIBOR to SOFR Disclosure" sheetId="16" r:id="rId11"/>
-    <sheet name="LEGAL DISCLAIMER" sheetId="11" r:id="rId12"/>
+    <sheet name="November_2025" sheetId="27" r:id="rId1"/>
+    <sheet name="October_2025" sheetId="26" r:id="rId2"/>
+    <sheet name="September_2025" sheetId="25" r:id="rId3"/>
+    <sheet name="August_2025" sheetId="24" r:id="rId4"/>
+    <sheet name="July_2025" sheetId="23" r:id="rId5"/>
+    <sheet name="June_2025" sheetId="22" r:id="rId6"/>
+    <sheet name="May_2025" sheetId="21" r:id="rId7"/>
+    <sheet name="April_2025" sheetId="20" r:id="rId8"/>
+    <sheet name="March_2025" sheetId="19" r:id="rId9"/>
+    <sheet name="February_2025" sheetId="18" r:id="rId10"/>
+    <sheet name="January_2025" sheetId="17" r:id="rId11"/>
+    <sheet name="LIBOR to SOFR Disclosure" sheetId="16" r:id="rId12"/>
+    <sheet name="LEGAL DISCLAIMER" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="21">
   <si>
     <t>Table J (01/31/2025) Swap Benchmark Spreads (in bps)</t>
   </si>
@@ -101,6 +102,9 @@
   </si>
   <si>
     <t>Table J (10/31/2025) Swap Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table J (11/28/2025) Swap Benchmark Spreads (in bps)</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1334,7 @@
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000008100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000008100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1651,7 +1655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379604C-B6E6-4443-AAC4-03BC4BA7C7BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6F2835-1535-437B-92EC-248A6371515D}">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1663,7 +1667,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1695,10 +1699,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="6">
-        <v>7.5452052592000003</v>
+        <v>-1.887906877</v>
       </c>
       <c r="C4" s="7">
-        <v>-8.7200979669999992</v>
+        <v>-8.6326097270000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,10 +1710,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>5.4702666666999997</v>
+        <v>1.7783312499999999</v>
       </c>
       <c r="C5" s="6">
-        <v>-19.285361930000001</v>
+        <v>-19.17339213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6">
-        <v>-4.7253047920000002</v>
+        <v>-6.8667596890000002</v>
       </c>
       <c r="C6" s="6">
-        <v>-6.640543954</v>
+        <v>-6.6292665910000004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1728,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="6">
-        <v>-17.986776559999999</v>
+        <v>-14.837141600000001</v>
       </c>
       <c r="C7" s="6">
-        <v>-9.4720105609999994</v>
+        <v>-9.5367021649999995</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,10 +1743,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>-22.139696440000002</v>
+        <v>-20.829166480000001</v>
       </c>
       <c r="C8" s="6">
-        <v>-13.59274679</v>
+        <v>-13.69393036</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1750,10 +1754,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="6">
-        <v>-24.92700718</v>
+        <v>-22.76229987</v>
       </c>
       <c r="C9" s="6">
-        <v>-17.683493819999999</v>
+        <v>-17.806993559999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1761,10 +1765,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="6">
-        <v>-27.975494569999999</v>
+        <v>-24.877004639999999</v>
       </c>
       <c r="C10" s="6">
-        <v>-20.650627650000001</v>
+        <v>-20.803627909999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,10 +1776,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>-31.868348059999999</v>
+        <v>-28.76618663</v>
       </c>
       <c r="C11" s="6">
-        <v>-23.018938479999999</v>
+        <v>-23.199092140000001</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1783,10 +1787,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="6">
-        <v>-35.12502439</v>
+        <v>-32.13687204</v>
       </c>
       <c r="C12" s="6">
-        <v>-24.643852169999999</v>
+        <v>-24.827642269999998</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1794,10 +1798,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="6">
-        <v>-37.41960933</v>
+        <v>-34.36064159</v>
       </c>
       <c r="C13" s="6">
-        <v>-25.804318949999999</v>
+        <v>-25.966189230000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,10 +1809,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="6">
-        <v>-39.25672204</v>
+        <v>-36.217203499999997</v>
       </c>
       <c r="C14" s="6">
-        <v>-26.708911199999999</v>
+        <v>-26.83723874</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,10 +1820,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="6">
-        <v>-40.73643036</v>
+        <v>-37.636845530000002</v>
       </c>
       <c r="C15" s="6">
-        <v>-27.496924369999999</v>
+        <v>-27.58993267</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,10 +1831,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="6">
-        <v>-42.903739680000001</v>
+        <v>-39.932199699999998</v>
       </c>
       <c r="C16" s="6">
-        <v>-28.461193489999999</v>
+        <v>-28.524672379999998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,10 +1842,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="6">
-        <v>-46.057547999999997</v>
+        <v>-43.440759329999999</v>
       </c>
       <c r="C17" s="6">
-        <v>-29.723373179999999</v>
+        <v>-29.76895309</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,10 +1853,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="6">
-        <v>-49.553482430000003</v>
+        <v>-47.18283701</v>
       </c>
       <c r="C18" s="6">
-        <v>-31.332886120000001</v>
+        <v>-31.36868042</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,10 +1864,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="6">
-        <v>-52.842691760000001</v>
+        <v>-50.577111940000002</v>
       </c>
       <c r="C19" s="6">
-        <v>-33.159291289999999</v>
+        <v>-33.190270419999997</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,10 +1875,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="6">
-        <v>-55.780143199999998</v>
+        <v>-53.492839099999998</v>
       </c>
       <c r="C20" s="6">
-        <v>-35.123963680000003</v>
+        <v>-35.153061600000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,10 +1886,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="6">
-        <v>-58.271733949999998</v>
+        <v>-56.023917300000001</v>
       </c>
       <c r="C21" s="6">
-        <v>-37.188682810000003</v>
+        <v>-37.218337740000003</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,10 +1897,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="6">
-        <v>-60.352144289999998</v>
+        <v>-58.055090569999997</v>
       </c>
       <c r="C22" s="6">
-        <v>-39.310638570000002</v>
+        <v>-39.341179740000001</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,10 +1908,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="6">
-        <v>-61.990687989999998</v>
+        <v>-59.645390429999999</v>
       </c>
       <c r="C23" s="6">
-        <v>-41.428346990000001</v>
+        <v>-41.460715399999998</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,10 +1919,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="6">
-        <v>-63.199702420000001</v>
+        <v>-60.875489780000002</v>
       </c>
       <c r="C24" s="6">
-        <v>-43.484311140000003</v>
+        <v>-43.518742189999998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,10 +1930,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="6">
-        <v>-64.117122510000002</v>
+        <v>-61.792998410000003</v>
       </c>
       <c r="C25" s="6">
-        <v>-45.416549179999997</v>
+        <v>-45.453901119999998</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,10 +1941,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="6">
-        <v>-64.765575459999994</v>
+        <v>-62.507469839999999</v>
       </c>
       <c r="C26" s="6">
-        <v>-47.262596160000001</v>
+        <v>-47.303131319999999</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,10 +1952,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="6">
-        <v>-65.339519980000006</v>
+        <v>-63.138604659999999</v>
       </c>
       <c r="C27" s="6">
-        <v>-49.034732159999997</v>
+        <v>-49.077808040000001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,10 +1963,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="6">
-        <v>-65.845528860000002</v>
+        <v>-63.692138669999999</v>
       </c>
       <c r="C28" s="6">
-        <v>-50.658714289999999</v>
+        <v>-50.70311641</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,10 +1974,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="6">
-        <v>-66.293890239999996</v>
+        <v>-64.249029350000001</v>
       </c>
       <c r="C29" s="6">
-        <v>-52.071209860000003</v>
+        <v>-52.115476839999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,10 +1985,10 @@
         <v>25</v>
       </c>
       <c r="B30" s="6">
-        <v>-66.744520050000006</v>
+        <v>-64.798857859999998</v>
       </c>
       <c r="C30" s="6">
-        <v>-53.212020039999999</v>
+        <v>-53.254990900000003</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,10 +1996,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="6">
-        <v>-67.180333259999998</v>
+        <v>-65.321158749999995</v>
       </c>
       <c r="C31" s="6">
-        <v>-54.048755929999999</v>
+        <v>-54.088753140000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,10 +2007,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="6">
-        <v>-67.661478500000001</v>
+        <v>-65.835949240000005</v>
       </c>
       <c r="C32" s="6">
-        <v>-54.596377570000001</v>
+        <v>-54.630743340000002</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,10 +2018,10 @@
         <v>28</v>
       </c>
       <c r="B33" s="6">
-        <v>-68.135175320000002</v>
+        <v>-66.429597860000001</v>
       </c>
       <c r="C33" s="6">
-        <v>-54.856236529999997</v>
+        <v>-54.882454289999998</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2025,10 +2029,10 @@
         <v>29</v>
       </c>
       <c r="B34" s="6">
-        <v>-68.615861069999994</v>
+        <v>-67.028187279999997</v>
       </c>
       <c r="C34" s="6">
-        <v>-54.826682030000001</v>
+        <v>-54.841728379999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2036,10 +2040,10 @@
         <v>30</v>
       </c>
       <c r="B35" s="6">
-        <v>-69.238849970000004</v>
+        <v>-67.757695569999996</v>
       </c>
       <c r="C35" s="6">
-        <v>-54.546699580000002</v>
+        <v>-54.54834915</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2047,10 +2051,10 @@
         <v>8</v>
       </c>
       <c r="B36" s="8">
-        <v>-46.688583460503118</v>
+        <v>-45.036781870187504</v>
       </c>
       <c r="C36" s="8">
-        <v>-34.795659013812497</v>
+        <v>-34.848177606343747</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2076,6 +2080,432 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A43502-C709-47ED-82F5-620B67AC7AF2}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6">
+        <v>8.3710618562000008</v>
+      </c>
+      <c r="C4" s="7">
+        <v>-9.1223835040000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6.8827604167000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-20.07372711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>-0.45804236300000001</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-6.7572968769999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-12.71941795</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-8.8279884079999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-20.15243714</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-12.588669919999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-23.751924819999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-16.554409629999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-27.194243180000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>-19.512283499999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-32.489066280000003</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-21.90164253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-36.337831289999997</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-23.653459680000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-38.706014519999997</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-25.049233730000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-40.471754949999998</v>
+      </c>
+      <c r="C14" s="6">
+        <v>-26.202677690000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-42.00349147</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-27.206369429999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="6">
+        <v>-44.176867280000003</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-28.301749300000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6">
+        <v>-46.912354790000002</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-29.595148940000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-49.899324960000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-31.164094469999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-52.964594329999997</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-32.906071109999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-55.842553180000003</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-34.769279509999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6">
+        <v>-58.401681119999999</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-36.734082770000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>17</v>
+      </c>
+      <c r="B22" s="6">
+        <v>-60.589063639999999</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-38.767443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6">
+        <v>-62.395214369999998</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-40.803412960000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>19</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-63.906038039999999</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-42.78701478</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="6">
+        <v>-65.080182550000004</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-44.652505580000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6">
+        <v>-66.067297150000002</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-46.43781911</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6">
+        <v>-67.064761509999997</v>
+      </c>
+      <c r="C27" s="6">
+        <v>-48.159291840000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6">
+        <v>-68.000502510000004</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-49.745504920000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6">
+        <v>-68.888497229999999</v>
+      </c>
+      <c r="C29" s="6">
+        <v>-51.13243095</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>25</v>
+      </c>
+      <c r="B30" s="6">
+        <v>-69.799231989999996</v>
+      </c>
+      <c r="C30" s="6">
+        <v>-52.258362290000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>26</v>
+      </c>
+      <c r="B31" s="6">
+        <v>-70.670586290000003</v>
+      </c>
+      <c r="C31" s="6">
+        <v>-53.092458290000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6">
+        <v>-71.565499059999993</v>
+      </c>
+      <c r="C32" s="6">
+        <v>-53.656817369999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>28</v>
+      </c>
+      <c r="B33" s="6">
+        <v>-72.464189930000003</v>
+      </c>
+      <c r="C33" s="6">
+        <v>-53.951834089999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>29</v>
+      </c>
+      <c r="B34" s="6">
+        <v>-73.397111649999999</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-53.977415229999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>30</v>
+      </c>
+      <c r="B35" s="6">
+        <v>-74.446040249999996</v>
+      </c>
+      <c r="C35" s="6">
+        <v>-53.770619439999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="8">
+        <v>-47.548812297503126</v>
+      </c>
+      <c r="C36" s="8">
+        <v>-34.191046811218747</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A39:E39"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0334E61F-4137-42F1-8ADC-1EC55566A90B}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E39"/>
@@ -2501,7 +2931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25262A5-84B2-4BF6-AF4E-DBAA1AC8379B}">
   <sheetPr codeName="Sheet8">
     <tabColor rgb="FFFFFF00"/>
@@ -2517,7 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FFFFFF00"/>
@@ -2568,6 +2998,431 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379604C-B6E6-4443-AAC4-03BC4BA7C7BE}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6">
+        <v>7.5452052592000003</v>
+      </c>
+      <c r="C4" s="7">
+        <v>-8.7200979669999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5.4702666666999997</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-19.285361930000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>-4.7253047920000002</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-6.640543954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-17.986776559999999</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-9.4720105609999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-22.139696440000002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-13.59274679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-24.92700718</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-17.683493819999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-27.975494569999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>-20.650627650000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-31.868348059999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-23.018938479999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-35.12502439</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-24.643852169999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-37.41960933</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-25.804318949999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-39.25672204</v>
+      </c>
+      <c r="C14" s="6">
+        <v>-26.708911199999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-40.73643036</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-27.496924369999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="6">
+        <v>-42.903739680000001</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-28.461193489999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6">
+        <v>-46.057547999999997</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-29.723373179999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-49.553482430000003</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-31.332886120000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-52.842691760000001</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-33.159291289999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-55.780143199999998</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-35.123963680000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6">
+        <v>-58.271733949999998</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-37.188682810000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>17</v>
+      </c>
+      <c r="B22" s="6">
+        <v>-60.352144289999998</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-39.310638570000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6">
+        <v>-61.990687989999998</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-41.428346990000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>19</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-63.199702420000001</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-43.484311140000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="6">
+        <v>-64.117122510000002</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-45.416549179999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6">
+        <v>-64.765575459999994</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-47.262596160000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6">
+        <v>-65.339519980000006</v>
+      </c>
+      <c r="C27" s="6">
+        <v>-49.034732159999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6">
+        <v>-65.845528860000002</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-50.658714289999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6">
+        <v>-66.293890239999996</v>
+      </c>
+      <c r="C29" s="6">
+        <v>-52.071209860000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>25</v>
+      </c>
+      <c r="B30" s="6">
+        <v>-66.744520050000006</v>
+      </c>
+      <c r="C30" s="6">
+        <v>-53.212020039999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>26</v>
+      </c>
+      <c r="B31" s="6">
+        <v>-67.180333259999998</v>
+      </c>
+      <c r="C31" s="6">
+        <v>-54.048755929999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6">
+        <v>-67.661478500000001</v>
+      </c>
+      <c r="C32" s="6">
+        <v>-54.596377570000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>28</v>
+      </c>
+      <c r="B33" s="6">
+        <v>-68.135175320000002</v>
+      </c>
+      <c r="C33" s="6">
+        <v>-54.856236529999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>29</v>
+      </c>
+      <c r="B34" s="6">
+        <v>-68.615861069999994</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-54.826682030000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>30</v>
+      </c>
+      <c r="B35" s="6">
+        <v>-69.238849970000004</v>
+      </c>
+      <c r="C35" s="6">
+        <v>-54.546699580000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="8">
+        <v>-46.688583460503118</v>
+      </c>
+      <c r="C36" s="8">
+        <v>-34.795659013812497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A39:E39"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53624B2-29FC-4CB9-A7C6-D02151E5E76D}">
   <dimension ref="A1:E39"/>
   <sheetViews>
@@ -2992,7 +3847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1BF4C2-4434-4B4D-94BE-B91D2B1C25FB}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E39"/>
@@ -3418,7 +4273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB6296-F480-49B2-B4EA-61908574360C}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E39"/>
@@ -3844,7 +4699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE138FB-FABF-4565-91D3-7A1FC3DB0D62}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E39"/>
@@ -4270,7 +5125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A65C64-A2BC-4A28-9AE0-4ADFC897F100}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E39"/>
@@ -4696,7 +5551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36971AA9-8593-40CA-AF5E-AB605D9DEDA6}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E39"/>
@@ -5122,7 +5977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00F7CDB-E2F7-42FB-8E4C-712A9F309635}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E39"/>
@@ -5546,430 +6401,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A43502-C709-47ED-82F5-620B67AC7AF2}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:E39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="19.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6">
-        <v>8.3710618562000008</v>
-      </c>
-      <c r="C4" s="7">
-        <v>-9.1223835040000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6.8827604167000001</v>
-      </c>
-      <c r="C5" s="6">
-        <v>-20.07372711</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>-0.45804236300000001</v>
-      </c>
-      <c r="C6" s="6">
-        <v>-6.7572968769999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6">
-        <v>-12.71941795</v>
-      </c>
-      <c r="C7" s="6">
-        <v>-8.8279884079999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6">
-        <v>-20.15243714</v>
-      </c>
-      <c r="C8" s="6">
-        <v>-12.588669919999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6">
-        <v>-23.751924819999999</v>
-      </c>
-      <c r="C9" s="6">
-        <v>-16.554409629999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6">
-        <v>-27.194243180000001</v>
-      </c>
-      <c r="C10" s="6">
-        <v>-19.512283499999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>6</v>
-      </c>
-      <c r="B11" s="6">
-        <v>-32.489066280000003</v>
-      </c>
-      <c r="C11" s="6">
-        <v>-21.90164253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6">
-        <v>-36.337831289999997</v>
-      </c>
-      <c r="C12" s="6">
-        <v>-23.653459680000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>8</v>
-      </c>
-      <c r="B13" s="6">
-        <v>-38.706014519999997</v>
-      </c>
-      <c r="C13" s="6">
-        <v>-25.049233730000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>9</v>
-      </c>
-      <c r="B14" s="6">
-        <v>-40.471754949999998</v>
-      </c>
-      <c r="C14" s="6">
-        <v>-26.202677690000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6">
-        <v>-42.00349147</v>
-      </c>
-      <c r="C15" s="6">
-        <v>-27.206369429999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>11</v>
-      </c>
-      <c r="B16" s="6">
-        <v>-44.176867280000003</v>
-      </c>
-      <c r="C16" s="6">
-        <v>-28.301749300000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>12</v>
-      </c>
-      <c r="B17" s="6">
-        <v>-46.912354790000002</v>
-      </c>
-      <c r="C17" s="6">
-        <v>-29.595148940000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>13</v>
-      </c>
-      <c r="B18" s="6">
-        <v>-49.899324960000001</v>
-      </c>
-      <c r="C18" s="6">
-        <v>-31.164094469999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6">
-        <v>-52.964594329999997</v>
-      </c>
-      <c r="C19" s="6">
-        <v>-32.906071109999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6">
-        <v>-55.842553180000003</v>
-      </c>
-      <c r="C20" s="6">
-        <v>-34.769279509999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>16</v>
-      </c>
-      <c r="B21" s="6">
-        <v>-58.401681119999999</v>
-      </c>
-      <c r="C21" s="6">
-        <v>-36.734082770000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>17</v>
-      </c>
-      <c r="B22" s="6">
-        <v>-60.589063639999999</v>
-      </c>
-      <c r="C22" s="6">
-        <v>-38.767443</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>18</v>
-      </c>
-      <c r="B23" s="6">
-        <v>-62.395214369999998</v>
-      </c>
-      <c r="C23" s="6">
-        <v>-40.803412960000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>19</v>
-      </c>
-      <c r="B24" s="6">
-        <v>-63.906038039999999</v>
-      </c>
-      <c r="C24" s="6">
-        <v>-42.78701478</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>20</v>
-      </c>
-      <c r="B25" s="6">
-        <v>-65.080182550000004</v>
-      </c>
-      <c r="C25" s="6">
-        <v>-44.652505580000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>21</v>
-      </c>
-      <c r="B26" s="6">
-        <v>-66.067297150000002</v>
-      </c>
-      <c r="C26" s="6">
-        <v>-46.43781911</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>22</v>
-      </c>
-      <c r="B27" s="6">
-        <v>-67.064761509999997</v>
-      </c>
-      <c r="C27" s="6">
-        <v>-48.159291840000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>23</v>
-      </c>
-      <c r="B28" s="6">
-        <v>-68.000502510000004</v>
-      </c>
-      <c r="C28" s="6">
-        <v>-49.745504920000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>24</v>
-      </c>
-      <c r="B29" s="6">
-        <v>-68.888497229999999</v>
-      </c>
-      <c r="C29" s="6">
-        <v>-51.13243095</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>25</v>
-      </c>
-      <c r="B30" s="6">
-        <v>-69.799231989999996</v>
-      </c>
-      <c r="C30" s="6">
-        <v>-52.258362290000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>26</v>
-      </c>
-      <c r="B31" s="6">
-        <v>-70.670586290000003</v>
-      </c>
-      <c r="C31" s="6">
-        <v>-53.092458290000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>27</v>
-      </c>
-      <c r="B32" s="6">
-        <v>-71.565499059999993</v>
-      </c>
-      <c r="C32" s="6">
-        <v>-53.656817369999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6">
-        <v>-72.464189930000003</v>
-      </c>
-      <c r="C33" s="6">
-        <v>-53.951834089999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>29</v>
-      </c>
-      <c r="B34" s="6">
-        <v>-73.397111649999999</v>
-      </c>
-      <c r="C34" s="6">
-        <v>-53.977415229999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>30</v>
-      </c>
-      <c r="B35" s="6">
-        <v>-74.446040249999996</v>
-      </c>
-      <c r="C35" s="6">
-        <v>-53.770619439999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="8">
-        <v>-47.548812297503126</v>
-      </c>
-      <c r="C36" s="8">
-        <v>-34.191046811218747</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A39:E39"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>